<commit_message>
lo deje más bonito
</commit_message>
<xml_diff>
--- a/data/dinamicas.xlsx
+++ b/data/dinamicas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Montserrat\Documents\UC\5tosemestre\OFG\bitacora\bit-cora_juegos\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\softaff\bit-cora_juegos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D348B11E-37BD-42D8-8A39-022B9CAE6C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4F121D-1C22-4A9C-A201-6BAD88049B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{41D50509-63A5-1C4D-BBC4-5E8D78010E3B}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{41D50509-63A5-1C4D-BBC4-5E8D78010E3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -47,115 +47,49 @@
     <t>Esquema/dibujo/video</t>
   </si>
   <si>
-    <t>Canción del marciano</t>
-  </si>
-  <si>
-    <t>Saludo del marciano</t>
-  </si>
-  <si>
     <t>Catapum chimplún (bis) guriguriguriguri zoom zoom zoom.</t>
-  </si>
-  <si>
-    <t>El noble duque Juan</t>
   </si>
   <si>
     <t>El noble duque Juan, tenía hombres mil, subía la montaña y bajaba otra vez. Cuando sube sube sube, cuando baja baja baja y en medio del camino sube usted y bajo yo.</t>
   </si>
   <si>
-    <t>Palo palito</t>
-  </si>
-  <si>
     <t>Palo palo palo palo palito palo eh eh eh eh, palo palito palo eh.</t>
-  </si>
-  <si>
-    <t>Un elefante se balanceaba</t>
   </si>
   <si>
     <t>n elefantes se balanceaban sobre la tela de una araña, como veían que resistía fueron a buscar a otro elefante.</t>
   </si>
   <si>
-    <t>Soy capitán</t>
-  </si>
-  <si>
     <t>Soy capitán de un buque inglés y en cada puerto tengo una mujer la rubia es sensacional y la morena no está nada mal. Si alguna vez me iré a casar, me casaré con la que me guste más.</t>
-  </si>
-  <si>
-    <t>La sandía</t>
-  </si>
-  <si>
-    <t>Tallarín</t>
   </si>
   <si>
     <t>Un tallarín, un tallarín que se mueve por aquí, que se mueve por allá. Todo pegoteado, con un poco de aceite, con un poco de sal. Y te lo comes tú y sales a bailar.</t>
   </si>
   <si>
-    <t>El alacrán</t>
-  </si>
-  <si>
     <t>El alacrán, el alacrán. Cómo mueve su patita sí señor, cómo mueve su colita sí señor. Se mata así, se mata así, se mata así así y así.</t>
-  </si>
-  <si>
-    <t>Soy una taza</t>
   </si>
   <si>
     <t>Soy una taza, una tetera, una cuchara y un cucharón. Soy un plato plano, un plato hondo, un cuchillito y un tenedor. Soy un salero tss tss tss, azucarero tss tss tss, y ahora saca a tu compañero.</t>
   </si>
   <si>
-    <t>La familia pato</t>
-  </si>
-  <si>
-    <t>Limón y medio limón</t>
-  </si>
-  <si>
     <t>1 limón, medio limón, 2 limones</t>
-  </si>
-  <si>
-    <t>El pistón</t>
   </si>
   <si>
     <t>Es el pistón pistón el que hace andar a la máquina, es el pistón pistón que hace andar al vagón. x4</t>
   </si>
   <si>
-    <t>A moler café</t>
-  </si>
-  <si>
-    <t>Bugui Bugui</t>
-  </si>
-  <si>
     <t>Hey, bugui bugui, hey. (bis) Con la mano adentro, con la mano afuera. Con la mano adentro y la hacemos girar. Bailando el bugui bugui, una vuelta te darás.</t>
-  </si>
-  <si>
-    <t>El caracol</t>
   </si>
   <si>
     <t>Yo soy la amiguita del caracol que va dando vueltas más y mejor. Que pase por aquí lala, que pase por allá lala, hasta que encuentra la reina del sol. Le doy la mano, la miro así, después la saludo con mucha atención, le doy un abrazo más y mejor, sigamos la ronda del caracol.</t>
   </si>
   <si>
-    <t>El florín</t>
-  </si>
-  <si>
-    <t>One, two, three</t>
-  </si>
-  <si>
     <t>1,2,3 Frente, cara, mano, codo, punta, pie, señorita, caballero, compro un huevo, se me cae, lo recojo, me lo como, lo vomito, se acabó.</t>
-  </si>
-  <si>
-    <t>Rey de españa</t>
   </si>
   <si>
     <t>Este es el juego del rey de españa, más conocido como el hombre araña. ABC hula hula, ABC cha cha chá, ABC one two three.</t>
   </si>
   <si>
-    <t>Es un pasito</t>
-  </si>
-  <si>
     <t>Un paso aquí, un paso allá, es un pasito. Es un pasito por aquí y por allá.</t>
-  </si>
-  <si>
-    <t>Oh masa masa</t>
-  </si>
-  <si>
-    <t>Un árbol en el prado</t>
   </si>
   <si>
     <t>¿Por qué me sube la bilirrubina? ¡No sé! Otra vez, ¿Por qué me sube la bilirrubina? ¡No sé! A moler café, a moler café, a moler café...</t>
@@ -168,9 +102,6 @@
   </si>
   <si>
     <t>Links cloudinary</t>
-  </si>
-  <si>
-    <t>Larai lai lero</t>
   </si>
   <si>
     <t>Larai lai lero, larai lai lero, larai lai lero, lero lero lai.</t>
@@ -201,9 +132,6 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750375000/istockphoto-1274143774-612x612_htzmgs.jpg</t>
-  </si>
-  <si>
-    <t>Noé en su arca</t>
   </si>
   <si>
     <t>Un día Noé en su arca partió y muchos animales de 2 en 2 subió. Subió el cocodrilo y el orangután la picara serpiente el águila real. El conejo, el topo y el elefante loco loco loco eres tú.</t>
@@ -281,9 +209,6 @@
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750375004/piston-cartoon-260nw-390693694_fmxhhu.webp</t>
   </si>
   <si>
-    <t>El panadero</t>
-  </si>
-  <si>
     <t>¡Oh! Alele, alele. Alele quita tonga. Amasa, amasa, amasa. Oh aloé aloé aloá.</t>
   </si>
   <si>
@@ -344,9 +269,6 @@
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750374997/images_2_eoyo2t.jpg</t>
   </si>
   <si>
-    <t>Si las gotas de lluvia</t>
-  </si>
-  <si>
     <t>Si las gotas de lluvia fueran de caramelo, me encantaría estar ahí. Abriendo la boca para saborear, ah ah a-ah ah a-ah ah a-ah.</t>
   </si>
   <si>
@@ -354,9 +276,6 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750374987/91H2VKttszL._AC_UF894_1000_QL80__ccxapn.jpg</t>
-  </si>
-  <si>
-    <t>El sombrero</t>
   </si>
   <si>
     <t>El/La {nombre} le robó el sombrero al profesor. - ¿Quién yo? - Sí, tú. - Yo no fui. - ¿Quién fue? - ¡El/La {nombre}!</t>
@@ -368,9 +287,6 @@
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750375000/istockphoto-1364448487-612x612_wagjyi.jpg</t>
   </si>
   <si>
-    <t>La ensalada</t>
-  </si>
-  <si>
     <t>Este es el baile de la ensalada que está de moda y a ti te gusta. Atención. Preparar. El tomate, la lechuga, el pepino, la zanahoria.</t>
   </si>
   <si>
@@ -378,9 +294,6 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750374991/descarga_1_n7lcw2.jpg</t>
-  </si>
-  <si>
-    <t>Wanna</t>
   </si>
   <si>
     <t>Wanna. Wanana. Wana wana chuchu wana wana. Wan uno wan dos wan tres wanana. Wana wana chuchu wana wana.</t>
@@ -392,9 +305,6 @@
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750375002/ninos-abrazan-hacer-ronda_33070-5208_xpmqyb.avif</t>
   </si>
   <si>
-    <t>Cabeza boca</t>
-  </si>
-  <si>
     <t>Cabeza boca mano codo pie rodilla very one, two, three Medio paso very one, two, three</t>
   </si>
   <si>
@@ -402,9 +312,6 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750374994/f1bd0-poema2b4_hrxs5v.webp</t>
-  </si>
-  <si>
-    <t>El papá de Abraham</t>
   </si>
   <si>
     <t>El papá de Abraham tenía hijos, 7 hijos tenía el papá de Abraham. Que cuando cantaban, Que cuando reían, Hacían gestos como tú.</t>
@@ -416,9 +323,6 @@
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750375004/padre-hija-e-hijo_1308-3279_zuamsz.avif</t>
   </si>
   <si>
-    <t>Yo tengo una casita</t>
-  </si>
-  <si>
     <t>Yo tengo una casita, así así. Toco la puertita, así así. Abro las ventanas, así así, Y por la chimenea sale el humo, así así.</t>
   </si>
   <si>
@@ -426,9 +330,6 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750374989/casa-encantadora-ilustracion-arbol_1308-176337_a0xqth.avif</t>
-  </si>
-  <si>
-    <t>Pampa y cielo</t>
   </si>
   <si>
     <t>¡Paaampa y cielo! ¡Cieeelo y pampa! Y en el medio de la pampa, ¡un ñandú! Y al lado del ñandú, ¡un caballo! Y arriba del caballo, ¡un vaquero tomando mante! Y al lado del vaquero tomando mate, ¡un perro que mueve la cola!</t>
@@ -440,9 +341,6 @@
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750375001/istockphoto-1412263287-612x612_j5fzyp.jpg</t>
   </si>
   <si>
-    <t>Cha-cha slide</t>
-  </si>
-  <si>
     <t>Right foot, two stomps. Left foot, two stomps. Slide to the left. Slide to the right. Criss cross, criss cross. Cha cha real smooth.</t>
   </si>
   <si>
@@ -450,9 +348,6 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750374997/images_3_b9tfwg.jpg</t>
-  </si>
-  <si>
-    <t>Patos, pollos y gallinas</t>
   </si>
   <si>
     <t>Patos, pollos y gallinas van. Corriendo por el gallinero están. Perseguidos bárbaramente ¿por quién? Por el patrón poporopo, por el patrón poporopo.</t>
@@ -464,9 +359,6 @@
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750374986/178621460-duck-and-hen-with-chickens-farm-birds-poultry-breeding-cartoon-vector-illustration_o3cpwy.jpg</t>
   </si>
   <si>
-    <t>Soy una serpiente</t>
-  </si>
-  <si>
     <t>Soy una serpiente que anda por el bosque. Buscando una parte de su cola. ¿Quiere ser usted una parte de mi cola?</t>
   </si>
   <si>
@@ -474,9 +366,6 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750374987/192995395-cartoon-illustration-of-a-snake_jr7oab.jpg</t>
-  </si>
-  <si>
-    <t>Yo tengo un tick</t>
   </si>
   <si>
     <t>Yo tengo un tick tick tick (bis). El doctor me dijo que no tengo nada, pero estoy seguro que yo tengo un tick tick tick.</t>
@@ -488,16 +377,10 @@
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750374986/5cfa269ea8980903571c33d04c4cd879_si6dmc.jpg</t>
   </si>
   <si>
-    <t>Merequetengue</t>
-  </si>
-  <si>
     <t>Merequetengue tengue tengue, merequetengue tengue tengue tengue tengue.</t>
   </si>
   <si>
     <t>https://youtu.be/fm_tZKLkiJM?si=a6xKW3H_xsMIYtjW</t>
-  </si>
-  <si>
-    <t>Café con leche</t>
   </si>
   <si>
     <t>Café. Café con leche, café. Chocolate con ensaimada le gusta a usted, le gusta a usted. Y ahora que estamos solos y ahora que nadie nos ve: arriba la cafetera con el café, con el café.</t>
@@ -509,9 +392,6 @@
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750375963/images_5_ld8snq.jpg</t>
   </si>
   <si>
-    <t>Chuchuwá</t>
-  </si>
-  <si>
     <t>¡Compañía! Brazo extendido, puño cerrado, pulgar hacia arriba, hombros caídos, cabeza hacia atrás, cola hacia atrás, pie de pingüino, lengua afuera. Chuchuwá, chuchuwá, chuchuwá wa wa.</t>
   </si>
   <si>
@@ -521,16 +401,10 @@
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750374987/ab67616d0000b2736a61be7ce315c0a750626f16_xtslty.jpg</t>
   </si>
   <si>
-    <t>A la u</t>
-  </si>
-  <si>
     <t>A la u. A la u chicau. A la u, chicahuaca chicahuaca chicau. Aja, oh yes, esta vez</t>
   </si>
   <si>
     <t>https://youtu.be/wEamqy7geDE</t>
-  </si>
-  <si>
-    <t>Familia Sapo</t>
   </si>
   <si>
     <t>Estaba la familia sapo. Estaba el papá sapo, sucu sucu sucu sa, saa, saa. (Se repite cambiando el miembro familiar por mamá sapo, hijo sapo, hija sapo, bebé sapo)</t>
@@ -542,16 +416,10 @@
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750374998/images_4_wnn6yg.jpg</t>
   </si>
   <si>
-    <t>Todo el movimiento</t>
-  </si>
-  <si>
     <t>Todo el movimiento baila, baila, baila. Baila, baila, baila todo el movimiento. Con el pie pie, con el otro pie. Con el codo codo, con el otro codo, con la mano mano, con la otra mano, con el dedo dedo, con el otro dedo.</t>
   </si>
   <si>
     <t>https://youtu.be/iCWlJiIRE4U?si=7Mo3WKhGX-_P-XdJ</t>
-  </si>
-  <si>
-    <t>La vaca</t>
   </si>
   <si>
     <t>La vaca, la vaca. La vaca, la vaca, la vaca. Tiene colita, tiene pezuñas, tiene rodillas, tiene tetillas, tiene cuernitos.</t>
@@ -563,9 +431,6 @@
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750374991/descarga_2_djklrt.jpg</t>
   </si>
   <si>
-    <t>Hey hey, Superman</t>
-  </si>
-  <si>
     <t>Hey, hey Superman. (bis) ¿Y cómo hace? Él hace así. Ucha acha, ucha ucha acha, pero ucha acha, ucha ucha acha.</t>
   </si>
   <si>
@@ -573,9 +438,6 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750374992/descarga_gowkkf.png</t>
-  </si>
-  <si>
-    <t>Baile de la cebolla</t>
   </si>
   <si>
     <t>Este es el baile de la cebolla (bis). Primero la pelas y después a la olla. Si la cebolla te hace llorar, levanta las manos y ponte a bailar.</t>
@@ -587,9 +449,6 @@
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750375004/pngtree-cute-onion-characters-illustration-a-kawaii-vegetable-trio-png-image_15774698_cjfq7a.png</t>
   </si>
   <si>
-    <t>Yo tengo un tren</t>
-  </si>
-  <si>
     <t>- Yo tengo un tren que va para arriba - Yo tengo un tren que va para abajo (bis). - Para arriba - Para abajo (bis). - Para arriba, para arriba, para arriba. - Para abajo, para abajo, para abajo.</t>
   </si>
   <si>
@@ -597,9 +456,6 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750374986/7628485_ac0b1d.png</t>
-  </si>
-  <si>
-    <t>El gran guerrero</t>
   </si>
   <si>
     <t>Eh, ahí un gran guerrero. ¿Cómo le hace el gran guerrero? Eh, oe, oe oe oe.</t>
@@ -611,9 +467,6 @@
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750375002/medieval-knight-armor-vector-illustration-600nw-2478603485_gf0ktq.webp</t>
   </si>
   <si>
-    <t>Una flor</t>
-  </si>
-  <si>
     <t>Había una vez, pero había una vez, una flor en un jardín. Con ejercicio, uno dos, tres cuatro. ¡Más abajo!</t>
   </si>
   <si>
@@ -623,9 +476,6 @@
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750374999/images_olowzw.png</t>
   </si>
   <si>
-    <t>8 monitos</t>
-  </si>
-  <si>
     <t>8 monitos se fueron de paseo, haciéndole muecas al cocodrilo. ¡A que no me atrapas, a que no me atrapas! ¡Pero a que no me atrapas, a que no me atrapas! Y el cocodrilo muy hambriento, da un paso muy despacio. Y ¡zas! se come a uno y ¡zas! se come al otro. ¿Cuántos monitos quedan?</t>
   </si>
   <si>
@@ -633,6 +483,156 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/dqcokurje/image/upload/v1750374990/depositphotos_61153911-stock-illustration-cute-funny-monkeys_ly14ss.webp</t>
+  </si>
+  <si>
+    <t>🥁 Larai lai lero</t>
+  </si>
+  <si>
+    <t>👽🎵 Canción del marciano</t>
+  </si>
+  <si>
+    <t>👽👋 Saludo del marciano</t>
+  </si>
+  <si>
+    <t>🤴 El noble duque Juan</t>
+  </si>
+  <si>
+    <t>🛶 Noé en su arca</t>
+  </si>
+  <si>
+    <t>🌳 Palo palito</t>
+  </si>
+  <si>
+    <t>🐘 Un elefante se balanceaba</t>
+  </si>
+  <si>
+    <t>⚓ Soy capitán</t>
+  </si>
+  <si>
+    <t>🍉 La sandía</t>
+  </si>
+  <si>
+    <t>🍝 Tallarín</t>
+  </si>
+  <si>
+    <t>🦂 El alacrán</t>
+  </si>
+  <si>
+    <t>☕🍽️ Soy una taza</t>
+  </si>
+  <si>
+    <t>🦆👨‍👩‍👧‍👦 La familia pato</t>
+  </si>
+  <si>
+    <t>🍋 Limón y medio limón</t>
+  </si>
+  <si>
+    <t>🚗💨 El pistón</t>
+  </si>
+  <si>
+    <t>🥖👨‍🍳 El panadero</t>
+  </si>
+  <si>
+    <t>☕ A moler café</t>
+  </si>
+  <si>
+    <t>💃🌀 Bugui Bugui</t>
+  </si>
+  <si>
+    <t>🐌 El caracol</t>
+  </si>
+  <si>
+    <t>💃🕺 El florín</t>
+  </si>
+  <si>
+    <t>🔢 One, two, three</t>
+  </si>
+  <si>
+    <t>👑🇪🇸 Rey de España</t>
+  </si>
+  <si>
+    <t>👣 Es un pasito</t>
+  </si>
+  <si>
+    <t>🫱🍞🫲 Oh masa masa</t>
+  </si>
+  <si>
+    <t>🌳 Un árbol en el prado</t>
+  </si>
+  <si>
+    <t>☔🎶 Si las gotas de lluvia</t>
+  </si>
+  <si>
+    <t>🎩🪄 El sombrero</t>
+  </si>
+  <si>
+    <t>🥗🍅🥕 La ensalada</t>
+  </si>
+  <si>
+    <t>💃🎧 Wanna</t>
+  </si>
+  <si>
+    <t>🧠👄 Cabeza boca</t>
+  </si>
+  <si>
+    <t>👴👶🇮🇱 El papá de Abraham</t>
+  </si>
+  <si>
+    <t>🏠🎶 Yo tengo una casita</t>
+  </si>
+  <si>
+    <t>🏜️🌌 Pampa y cielo</t>
+  </si>
+  <si>
+    <t>🕺👣🎶 Cha-cha slide</t>
+  </si>
+  <si>
+    <t>🦆🐤🐔 Patos, pollos y gallinas</t>
+  </si>
+  <si>
+    <t>🐍🎶 Soy una serpiente</t>
+  </si>
+  <si>
+    <t>🤪 Yo tengo un tick</t>
+  </si>
+  <si>
+    <t>💃 Merequetengue</t>
+  </si>
+  <si>
+    <t>☕🥛 Café con leche</t>
+  </si>
+  <si>
+    <t>🕺🎶 Chuchuwá</t>
+  </si>
+  <si>
+    <t>🎓📣 A la u</t>
+  </si>
+  <si>
+    <t>🐸👨‍👩‍👧‍👦 Familia Sapo</t>
+  </si>
+  <si>
+    <t>🕺🌀 Todo el movimiento</t>
+  </si>
+  <si>
+    <t>🐄 La vaca</t>
+  </si>
+  <si>
+    <t>🦸‍♂️ Hey hey, Superman</t>
+  </si>
+  <si>
+    <t>🧅🕺 Baile de la cebolla</t>
+  </si>
+  <si>
+    <t>🚂 Yo tengo un tren</t>
+  </si>
+  <si>
+    <t>⚔️ El gran guerrero</t>
+  </si>
+  <si>
+    <t>🌸 Una flor</t>
+  </si>
+  <si>
+    <t>🐒 8 monitos</t>
   </si>
 </sst>
 </file>
@@ -1080,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F31B3D32-BD2A-8941-92F1-9434887BEF40}">
   <dimension ref="A1:Z1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A51" sqref="A2:A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1100,7 +1100,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -1127,16 +1127,16 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>44</v>
+        <v>149</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1163,16 +1163,16 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1199,16 +1199,16 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>151</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1235,16 +1235,16 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>152</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1271,16 +1271,16 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1307,16 +1307,16 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>8</v>
+        <v>154</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1343,16 +1343,16 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>10</v>
+        <v>155</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1379,16 +1379,16 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>156</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1415,16 +1415,16 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>14</v>
+        <v>157</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1451,16 +1451,16 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>15</v>
+        <v>158</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1487,16 +1487,16 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>17</v>
+        <v>159</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1523,16 +1523,16 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>19</v>
+        <v>160</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1559,16 +1559,16 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>161</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1595,16 +1595,16 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>162</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1631,16 +1631,16 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>24</v>
+        <v>163</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1667,16 +1667,16 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>81</v>
+        <v>164</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1703,16 +1703,16 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>26</v>
+        <v>165</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -1739,16 +1739,16 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>27</v>
+        <v>166</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1775,16 +1775,16 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>29</v>
+        <v>167</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1811,16 +1811,16 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>31</v>
+        <v>168</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -1847,16 +1847,16 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>32</v>
+        <v>169</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1883,16 +1883,16 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>34</v>
+        <v>170</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1919,16 +1919,16 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>36</v>
+        <v>171</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1955,16 +1955,16 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>38</v>
+        <v>172</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -1991,16 +1991,16 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>39</v>
+        <v>173</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -2027,16 +2027,16 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>102</v>
+        <v>174</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -2063,16 +2063,16 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>106</v>
+        <v>175</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -2099,16 +2099,16 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>110</v>
+        <v>176</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -2135,16 +2135,16 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>114</v>
+        <v>177</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>115</v>
+        <v>86</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -2171,16 +2171,16 @@
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>118</v>
+        <v>178</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -2207,16 +2207,16 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>122</v>
+        <v>179</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>123</v>
+        <v>92</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>124</v>
+        <v>93</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>125</v>
+        <v>94</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2243,16 +2243,16 @@
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>126</v>
+        <v>180</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -2279,16 +2279,16 @@
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>130</v>
+        <v>181</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>131</v>
+        <v>98</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>132</v>
+        <v>99</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>133</v>
+        <v>100</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -2315,16 +2315,16 @@
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>134</v>
+        <v>182</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>135</v>
+        <v>101</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -2351,16 +2351,16 @@
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>138</v>
+        <v>183</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>141</v>
+        <v>106</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -2387,16 +2387,16 @@
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>142</v>
+        <v>184</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>144</v>
+        <v>108</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>145</v>
+        <v>109</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -2423,16 +2423,16 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>146</v>
+        <v>185</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>148</v>
+        <v>111</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>149</v>
+        <v>112</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2459,16 +2459,16 @@
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>151</v>
+        <v>113</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>152</v>
+        <v>114</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -2495,16 +2495,16 @@
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>153</v>
+        <v>187</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>154</v>
+        <v>115</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>155</v>
+        <v>116</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>156</v>
+        <v>117</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -2531,16 +2531,16 @@
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>157</v>
+        <v>188</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>158</v>
+        <v>118</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>159</v>
+        <v>119</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -2567,16 +2567,16 @@
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>161</v>
+        <v>189</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>162</v>
+        <v>121</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>163</v>
+        <v>122</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -2603,16 +2603,16 @@
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>164</v>
+        <v>190</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>165</v>
+        <v>123</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>166</v>
+        <v>124</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>167</v>
+        <v>125</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -2639,16 +2639,16 @@
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>168</v>
+        <v>191</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>169</v>
+        <v>126</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>170</v>
+        <v>127</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -2675,16 +2675,16 @@
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>172</v>
+        <v>128</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>173</v>
+        <v>129</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>174</v>
+        <v>130</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -2711,16 +2711,16 @@
     </row>
     <row r="46" spans="1:26" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>175</v>
+        <v>193</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>176</v>
+        <v>131</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>177</v>
+        <v>132</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>178</v>
+        <v>133</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -2747,16 +2747,16 @@
     </row>
     <row r="47" spans="1:26" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>180</v>
+        <v>134</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>181</v>
+        <v>135</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>182</v>
+        <v>136</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -2783,16 +2783,16 @@
     </row>
     <row r="48" spans="1:26" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>184</v>
+        <v>137</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>185</v>
+        <v>138</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>186</v>
+        <v>139</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -2819,16 +2819,16 @@
     </row>
     <row r="49" spans="1:26" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>188</v>
+        <v>140</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>189</v>
+        <v>141</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>190</v>
+        <v>142</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -2855,16 +2855,16 @@
     </row>
     <row r="50" spans="1:26" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>192</v>
+        <v>143</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>193</v>
+        <v>144</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>194</v>
+        <v>145</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -2891,16 +2891,16 @@
     </row>
     <row r="51" spans="1:26" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>196</v>
+        <v>146</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>197</v>
+        <v>147</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>198</v>
+        <v>148</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>

</xml_diff>